<commit_message>
update 0.7 version output
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
+++ b/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
@@ -1649,14 +1649,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="37.94140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="37.9609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="84.15625" customWidth="true" bestFit="true"/>
@@ -1673,20 +1673,20 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="63.796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="74.484375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="74.52734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="33.40625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.57421875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="57.1953125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="57.25" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="70.45703125" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="33.046875" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
remove document bundles for pre-auth and pre-determination
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
+++ b/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="432">
   <si>
     <t>Property</t>
   </si>
@@ -1293,18 +1293,21 @@
     <t>claim</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Claim)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Claim.html)
 </t>
   </si>
   <si>
-    <t>A reference to the claim that the pre-auth request refers to.</t>
+    <t>A reference to the claim that the pre-determination/pre-authorization/claim request refers to.</t>
   </si>
   <si>
     <t>signature</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://raw.githubusercontent.com/Swasth-Digital-Health-Foundation/standards/69ce5ac4bc6e9fc5a015a53c82e3ebb7a379f348/FHIR%20Definitions/hcp.signature.extension.json)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-HCXSignatureExtension.html)
 </t>
+  </si>
+  <si>
+    <t>A reference to the signature in the pre-determination/pre-authorization/claim request refers to.</t>
   </si>
   <si>
     <t>Composition.section.emptyReason</t>
@@ -1659,7 +1662,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="84.15625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="87.26171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -7901,10 +7904,10 @@
         <v>417</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>407</v>
@@ -7989,7 +7992,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8015,16 +8018,16 @@
         <v>167</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>75</v>
@@ -8052,10 +8055,10 @@
         <v>110</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>75</v>
@@ -8073,7 +8076,7 @@
         <v>75</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>76</v>
@@ -8091,7 +8094,7 @@
         <v>75</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>163</v>
@@ -8105,7 +8108,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8131,13 +8134,13 @@
         <v>75</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -8187,7 +8190,7 @@
         <v>75</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>76</v>
@@ -8208,7 +8211,7 @@
         <v>355</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>75</v>

</xml_diff>

<commit_message>
update claim response doccument definition
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
+++ b/v0.7/StructureDefinition-ClaimRequestDocument.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="424">
   <si>
     <t>Property</t>
   </si>
@@ -1264,20 +1264,14 @@
     <t>Composition.section.entry</t>
   </si>
   <si>
-    <t>A reference to data that supports this section</t>
-  </si>
-  <si>
-    <t>A reference to the actual resource from which the narrative in the section is derived.</t>
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Claim.html)
+</t>
+  </si>
+  <si>
+    <t>A reference to the claim that the pre-determination/pre-authorization/claim request refers to.</t>
   </si>
   <si>
     <t>If there are no entries in the list, an emptyReason SHOULD be provided.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t xml:space="preserve">cmp-2
@@ -1288,26 +1282,6 @@
   </si>
   <si>
     <t>.entry</t>
-  </si>
-  <si>
-    <t>claim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Claim.html)
-</t>
-  </si>
-  <si>
-    <t>A reference to the claim that the pre-determination/pre-authorization/claim request refers to.</t>
-  </si>
-  <si>
-    <t>signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-HCXSignatureExtension.html)
-</t>
-  </si>
-  <si>
-    <t>A reference to the signature in the pre-determination/pre-authorization/claim request refers to.</t>
   </si>
   <si>
     <t>Composition.section.emptyReason</t>
@@ -1643,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN57"/>
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1662,7 +1636,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="87.26171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="85.484375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -7659,7 +7633,7 @@
         <v>86</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>75</v>
@@ -7671,10 +7645,10 @@
         <v>75</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>191</v>
+        <v>405</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>406</v>
@@ -7718,14 +7692,16 @@
         <v>75</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="AB53" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>75</v>
+      </c>
       <c r="AC53" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD53" t="s" s="2">
-        <v>409</v>
+        <v>75</v>
       </c>
       <c r="AE53" t="s" s="2">
         <v>404</v>
@@ -7737,7 +7713,7 @@
         <v>77</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>98</v>
@@ -7746,10 +7722,10 @@
         <v>75</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>75</v>
@@ -7760,17 +7736,15 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>413</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
         <v>75</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F54" t="s" s="2">
         <v>86</v>
@@ -7785,18 +7759,20 @@
         <v>75</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="K54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L54" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>75</v>
       </c>
@@ -7820,13 +7796,13 @@
         <v>75</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>75</v>
+        <v>416</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>75</v>
+        <v>417</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>75</v>
@@ -7844,16 +7820,16 @@
         <v>75</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>98</v>
@@ -7862,10 +7838,10 @@
         <v>75</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>412</v>
+        <v>163</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>75</v>
@@ -7876,11 +7852,9 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>416</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
         <v>75</v>
       </c>
@@ -7901,16 +7875,16 @@
         <v>75</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>417</v>
+        <v>75</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>407</v>
+        <v>422</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7960,7 +7934,7 @@
         <v>75</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>76</v>
@@ -7969,7 +7943,7 @@
         <v>77</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>98</v>
@@ -7978,245 +7952,15 @@
         <v>75</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>411</v>
+        <v>355</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="F56" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="G56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="H56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="I56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="J56" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="K56" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="O56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="P56" s="2"/>
-      <c r="Q56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="R56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="S56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="T56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="U56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="V56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="W56" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="X56" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="Y56" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AN56" t="s" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="F57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="H57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="I57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="J57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="K57" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="N57" s="2"/>
-      <c r="O57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="P57" s="2"/>
-      <c r="Q57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="R57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="S57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="T57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="U57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="V57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="W57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Z57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE57" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="AF57" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AG57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH57" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="AI57" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AN57" t="s" s="2">
         <v>75</v>
       </c>
     </row>

</xml_diff>